<commit_message>
csv updates May 7
</commit_message>
<xml_diff>
--- a/status/excel/fromBox/JORD_excel.xlsx
+++ b/status/excel/fromBox/JORD_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selenawallace/Documents/Data_Science/geography/status/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmccra01\Box\TFDD_Group_Shared\TFDD Data and Projects\Events Database\EventsUpdate2019_2023\Events Data Collection 2022-2023\Automation\Status Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3876584-1FDD-F24D-873B-74DA08310A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA4605B-7F4F-4F13-97B5-E30B6039C43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17500" yWindow="500" windowWidth="11300" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="360" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="month_loop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>index</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Jordan</t>
+  </si>
+  <si>
+    <t>06-30-2012</t>
   </si>
 </sst>
 </file>
@@ -638,9 +641,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -678,7 +681,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -784,7 +787,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -926,7 +929,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -936,18 +939,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="9" width="21.33203125" customWidth="1"/>
+    <col min="8" max="9" width="21.375" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -979,7 +982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -989,15 +992,15 @@
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3">
-        <v>39629</v>
-      </c>
-      <c r="E2" s="3">
-        <v>39994</v>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>41182</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1007,15 +1010,15 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3">
-        <v>39995</v>
-      </c>
-      <c r="E3" s="3">
-        <v>40359</v>
+      <c r="D3" s="1">
+        <v>41183</v>
+      </c>
+      <c r="E3" s="1">
+        <v>41274</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1025,15 +1028,15 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3">
-        <v>40360</v>
-      </c>
-      <c r="E4" s="3">
-        <v>40543</v>
+      <c r="D4" s="1">
+        <v>41275</v>
+      </c>
+      <c r="E4" s="1">
+        <v>41364</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1043,15 +1046,15 @@
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3">
-        <v>40544</v>
-      </c>
-      <c r="E5" s="3">
-        <v>40724</v>
+      <c r="D5" s="1">
+        <v>41365</v>
+      </c>
+      <c r="E5" s="1">
+        <v>41454</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1061,15 +1064,15 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3">
-        <v>40725</v>
-      </c>
-      <c r="E6" s="3">
-        <v>40816</v>
+      <c r="D6" s="1">
+        <v>45231</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45291</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1079,1502 +1082,1051 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3">
-        <v>40817</v>
-      </c>
-      <c r="E7" s="3">
-        <v>40908</v>
+      <c r="D7" s="1">
+        <v>45292</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45366</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3">
-        <v>40909</v>
-      </c>
-      <c r="E8" s="3">
-        <v>40999</v>
-      </c>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3">
-        <v>41000</v>
-      </c>
-      <c r="E9" s="3">
-        <v>41090</v>
-      </c>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1">
-        <v>41091</v>
-      </c>
-      <c r="E10" s="1">
-        <v>41182</v>
-      </c>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1">
-        <v>41183</v>
-      </c>
-      <c r="E11" s="1">
-        <v>41274</v>
-      </c>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1">
-        <v>41275</v>
-      </c>
-      <c r="E12" s="1">
-        <v>41364</v>
-      </c>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1">
-        <v>41365</v>
-      </c>
-      <c r="E13" s="1">
-        <v>41455</v>
-      </c>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1">
-        <v>41456</v>
-      </c>
-      <c r="E14" s="1">
-        <v>41547</v>
-      </c>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1">
-        <v>41548</v>
-      </c>
-      <c r="E15" s="1">
-        <v>41639</v>
-      </c>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1">
-        <v>41640</v>
-      </c>
-      <c r="E16" s="1">
-        <v>41729</v>
-      </c>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1">
-        <v>41730</v>
-      </c>
-      <c r="E17" s="1">
-        <v>41820</v>
-      </c>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1">
-        <v>41821</v>
-      </c>
-      <c r="E18" s="1">
-        <v>41912</v>
-      </c>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1">
-        <v>41913</v>
-      </c>
-      <c r="E19" s="1">
-        <v>42004</v>
-      </c>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1">
-        <v>42005</v>
-      </c>
-      <c r="E20" s="1">
-        <v>42094</v>
-      </c>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1">
-        <v>42095</v>
-      </c>
-      <c r="E21" s="1">
-        <v>42185</v>
-      </c>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="1">
-        <v>42186</v>
-      </c>
-      <c r="E22" s="1">
-        <v>42277</v>
-      </c>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1">
-        <v>42278</v>
-      </c>
-      <c r="E23" s="1">
-        <v>42369</v>
-      </c>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1">
-        <v>42370</v>
-      </c>
-      <c r="E24" s="1">
-        <v>42460</v>
-      </c>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1">
-        <v>42461</v>
-      </c>
-      <c r="E25" s="1">
-        <v>42551</v>
-      </c>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="1">
-        <v>42552</v>
-      </c>
-      <c r="E26" s="1">
-        <v>42643</v>
-      </c>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1">
-        <v>42644</v>
-      </c>
-      <c r="E27" s="1">
-        <v>42735</v>
-      </c>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="1">
-        <v>42736</v>
-      </c>
-      <c r="E28" s="1">
-        <v>42825</v>
-      </c>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1">
-        <v>42826</v>
-      </c>
-      <c r="E29" s="1">
-        <v>42916</v>
-      </c>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1">
-        <v>42917</v>
-      </c>
-      <c r="E30" s="1">
-        <v>43008</v>
-      </c>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="1">
-        <v>43009</v>
-      </c>
-      <c r="E31" s="1">
-        <v>43100</v>
-      </c>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="1">
-        <v>43101</v>
-      </c>
-      <c r="E32" s="1">
-        <v>43190</v>
-      </c>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="1">
-        <v>43191</v>
-      </c>
-      <c r="E33" s="1">
-        <v>43281</v>
-      </c>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="1">
-        <v>43282</v>
-      </c>
-      <c r="E34" s="1">
-        <v>43373</v>
-      </c>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1">
-        <v>43374</v>
-      </c>
-      <c r="E35" s="1">
-        <v>43465</v>
-      </c>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1">
-        <v>43466</v>
-      </c>
-      <c r="E36" s="1">
-        <v>43555</v>
-      </c>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1">
-        <v>43556</v>
-      </c>
-      <c r="E37" s="1">
-        <v>43646</v>
-      </c>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="1">
-        <v>43647</v>
-      </c>
-      <c r="E38" s="1">
-        <v>43830</v>
-      </c>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1">
-        <v>43831</v>
-      </c>
-      <c r="E39" s="1">
-        <v>44012</v>
-      </c>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="1">
-        <v>44013</v>
-      </c>
-      <c r="E40" s="1">
-        <v>44196</v>
-      </c>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="1">
-        <v>44197</v>
-      </c>
-      <c r="E41" s="1">
-        <v>44377</v>
-      </c>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="1">
-        <v>44378</v>
-      </c>
-      <c r="E42" s="1">
-        <v>44561</v>
-      </c>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>41</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="1">
-        <v>44562</v>
-      </c>
-      <c r="E43" s="1">
-        <v>44742</v>
-      </c>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>42</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="1">
-        <v>44743</v>
-      </c>
-      <c r="E44" s="1">
-        <v>44926</v>
-      </c>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>43</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="1">
-        <v>44927</v>
-      </c>
-      <c r="E45" s="1">
-        <v>45107</v>
-      </c>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="1">
-        <v>45108</v>
-      </c>
-      <c r="E46" s="1">
-        <v>45199</v>
-      </c>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>45</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="1">
-        <v>45200</v>
-      </c>
-      <c r="E47" s="1">
-        <v>45291</v>
-      </c>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>46</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="1">
-        <v>45292</v>
-      </c>
-      <c r="E48" s="1">
-        <v>45366</v>
-      </c>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F155" s="1"/>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F156" s="1"/>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F157" s="1"/>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F158" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
csv list May 7
</commit_message>
<xml_diff>
--- a/status/excel/fromBox/JORD_excel.xlsx
+++ b/status/excel/fromBox/JORD_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selenawallace/Documents/Data_Science/geography/status/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmccra01\Box\TFDD_Group_Shared\TFDD Data and Projects\Events Database\EventsUpdate2019_2023\Events Data Collection 2022-2023\Automation\Status Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3876584-1FDD-F24D-873B-74DA08310A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA4605B-7F4F-4F13-97B5-E30B6039C43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17500" yWindow="500" windowWidth="11300" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="360" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="month_loop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>index</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Jordan</t>
+  </si>
+  <si>
+    <t>06-30-2012</t>
   </si>
 </sst>
 </file>
@@ -638,9 +641,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -678,7 +681,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -784,7 +787,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -926,7 +929,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -936,18 +939,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="9" width="21.33203125" customWidth="1"/>
+    <col min="8" max="9" width="21.375" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -979,7 +982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -989,15 +992,15 @@
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3">
-        <v>39629</v>
-      </c>
-      <c r="E2" s="3">
-        <v>39994</v>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>41182</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1007,15 +1010,15 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3">
-        <v>39995</v>
-      </c>
-      <c r="E3" s="3">
-        <v>40359</v>
+      <c r="D3" s="1">
+        <v>41183</v>
+      </c>
+      <c r="E3" s="1">
+        <v>41274</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1025,15 +1028,15 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3">
-        <v>40360</v>
-      </c>
-      <c r="E4" s="3">
-        <v>40543</v>
+      <c r="D4" s="1">
+        <v>41275</v>
+      </c>
+      <c r="E4" s="1">
+        <v>41364</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1043,15 +1046,15 @@
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3">
-        <v>40544</v>
-      </c>
-      <c r="E5" s="3">
-        <v>40724</v>
+      <c r="D5" s="1">
+        <v>41365</v>
+      </c>
+      <c r="E5" s="1">
+        <v>41454</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1061,15 +1064,15 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3">
-        <v>40725</v>
-      </c>
-      <c r="E6" s="3">
-        <v>40816</v>
+      <c r="D6" s="1">
+        <v>45231</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45291</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1079,1502 +1082,1051 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3">
-        <v>40817</v>
-      </c>
-      <c r="E7" s="3">
-        <v>40908</v>
+      <c r="D7" s="1">
+        <v>45292</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45366</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3">
-        <v>40909</v>
-      </c>
-      <c r="E8" s="3">
-        <v>40999</v>
-      </c>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3">
-        <v>41000</v>
-      </c>
-      <c r="E9" s="3">
-        <v>41090</v>
-      </c>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1">
-        <v>41091</v>
-      </c>
-      <c r="E10" s="1">
-        <v>41182</v>
-      </c>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1">
-        <v>41183</v>
-      </c>
-      <c r="E11" s="1">
-        <v>41274</v>
-      </c>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1">
-        <v>41275</v>
-      </c>
-      <c r="E12" s="1">
-        <v>41364</v>
-      </c>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1">
-        <v>41365</v>
-      </c>
-      <c r="E13" s="1">
-        <v>41455</v>
-      </c>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1">
-        <v>41456</v>
-      </c>
-      <c r="E14" s="1">
-        <v>41547</v>
-      </c>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1">
-        <v>41548</v>
-      </c>
-      <c r="E15" s="1">
-        <v>41639</v>
-      </c>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1">
-        <v>41640</v>
-      </c>
-      <c r="E16" s="1">
-        <v>41729</v>
-      </c>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1">
-        <v>41730</v>
-      </c>
-      <c r="E17" s="1">
-        <v>41820</v>
-      </c>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1">
-        <v>41821</v>
-      </c>
-      <c r="E18" s="1">
-        <v>41912</v>
-      </c>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1">
-        <v>41913</v>
-      </c>
-      <c r="E19" s="1">
-        <v>42004</v>
-      </c>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1">
-        <v>42005</v>
-      </c>
-      <c r="E20" s="1">
-        <v>42094</v>
-      </c>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1">
-        <v>42095</v>
-      </c>
-      <c r="E21" s="1">
-        <v>42185</v>
-      </c>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="1">
-        <v>42186</v>
-      </c>
-      <c r="E22" s="1">
-        <v>42277</v>
-      </c>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1">
-        <v>42278</v>
-      </c>
-      <c r="E23" s="1">
-        <v>42369</v>
-      </c>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1">
-        <v>42370</v>
-      </c>
-      <c r="E24" s="1">
-        <v>42460</v>
-      </c>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1">
-        <v>42461</v>
-      </c>
-      <c r="E25" s="1">
-        <v>42551</v>
-      </c>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="1">
-        <v>42552</v>
-      </c>
-      <c r="E26" s="1">
-        <v>42643</v>
-      </c>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1">
-        <v>42644</v>
-      </c>
-      <c r="E27" s="1">
-        <v>42735</v>
-      </c>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="1">
-        <v>42736</v>
-      </c>
-      <c r="E28" s="1">
-        <v>42825</v>
-      </c>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1">
-        <v>42826</v>
-      </c>
-      <c r="E29" s="1">
-        <v>42916</v>
-      </c>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1">
-        <v>42917</v>
-      </c>
-      <c r="E30" s="1">
-        <v>43008</v>
-      </c>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="1">
-        <v>43009</v>
-      </c>
-      <c r="E31" s="1">
-        <v>43100</v>
-      </c>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="1">
-        <v>43101</v>
-      </c>
-      <c r="E32" s="1">
-        <v>43190</v>
-      </c>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="1">
-        <v>43191</v>
-      </c>
-      <c r="E33" s="1">
-        <v>43281</v>
-      </c>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="1">
-        <v>43282</v>
-      </c>
-      <c r="E34" s="1">
-        <v>43373</v>
-      </c>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1">
-        <v>43374</v>
-      </c>
-      <c r="E35" s="1">
-        <v>43465</v>
-      </c>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1">
-        <v>43466</v>
-      </c>
-      <c r="E36" s="1">
-        <v>43555</v>
-      </c>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1">
-        <v>43556</v>
-      </c>
-      <c r="E37" s="1">
-        <v>43646</v>
-      </c>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="1">
-        <v>43647</v>
-      </c>
-      <c r="E38" s="1">
-        <v>43830</v>
-      </c>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1">
-        <v>43831</v>
-      </c>
-      <c r="E39" s="1">
-        <v>44012</v>
-      </c>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="1">
-        <v>44013</v>
-      </c>
-      <c r="E40" s="1">
-        <v>44196</v>
-      </c>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="1">
-        <v>44197</v>
-      </c>
-      <c r="E41" s="1">
-        <v>44377</v>
-      </c>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="1">
-        <v>44378</v>
-      </c>
-      <c r="E42" s="1">
-        <v>44561</v>
-      </c>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>41</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="1">
-        <v>44562</v>
-      </c>
-      <c r="E43" s="1">
-        <v>44742</v>
-      </c>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>42</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="1">
-        <v>44743</v>
-      </c>
-      <c r="E44" s="1">
-        <v>44926</v>
-      </c>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>43</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="1">
-        <v>44927</v>
-      </c>
-      <c r="E45" s="1">
-        <v>45107</v>
-      </c>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="1">
-        <v>45108</v>
-      </c>
-      <c r="E46" s="1">
-        <v>45199</v>
-      </c>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>45</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="1">
-        <v>45200</v>
-      </c>
-      <c r="E47" s="1">
-        <v>45291</v>
-      </c>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>46</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="1">
-        <v>45292</v>
-      </c>
-      <c r="E48" s="1">
-        <v>45366</v>
-      </c>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F155" s="1"/>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F156" s="1"/>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F157" s="1"/>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F158" s="1"/>
     </row>
   </sheetData>

</xml_diff>